<commit_message>
Select windows for Actigraph data
</commit_message>
<xml_diff>
--- a/data/data_description_V2.xlsx
+++ b/data/data_description_V2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Work\sharedfolder\DATA\schudmachine\Data_mechanical_shaker_experiments_November2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annelindelettink/Documents/Work MacBook Pro Annelinde/Mechanical Shaker Machine/mechanicalshakerexperiments/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88BCACCF-1EB4-4345-B861-F04AA7B5DCF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CD12F0C-8BFF-6B4E-92B3-E82DC062D203}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="8385" windowWidth="29040" windowHeight="15840" tabRatio="1000" xr2:uid="{DFF87B92-3E22-ED4E-B7B8-2BEA09DD2480}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" tabRatio="1000" xr2:uid="{DFF87B92-3E22-ED4E-B7B8-2BEA09DD2480}"/>
   </bookViews>
   <sheets>
     <sheet name="activity_log" sheetId="4" r:id="rId1"/>
@@ -501,23 +501,23 @@
   <dimension ref="A1:K1048465"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="52.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
@@ -546,7 +546,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>2</v>
       </c>
@@ -575,7 +575,7 @@
         <v>0.40625</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -605,7 +605,7 @@
       </c>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -635,7 +635,7 @@
       </c>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>2</v>
       </c>
@@ -665,7 +665,7 @@
       </c>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>2</v>
       </c>
@@ -695,7 +695,7 @@
       </c>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>2</v>
       </c>
@@ -725,7 +725,7 @@
       </c>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>2</v>
       </c>
@@ -755,7 +755,7 @@
       </c>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>2</v>
       </c>
@@ -785,7 +785,7 @@
       </c>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>2</v>
       </c>
@@ -815,7 +815,7 @@
       </c>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>2</v>
       </c>
@@ -845,7 +845,7 @@
       </c>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>2</v>
       </c>
@@ -875,7 +875,7 @@
       </c>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
         <v>2</v>
       </c>
@@ -905,7 +905,7 @@
       </c>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>2</v>
       </c>
@@ -935,7 +935,7 @@
       </c>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
         <v>2</v>
       </c>
@@ -965,7 +965,7 @@
       </c>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
         <v>2</v>
       </c>
@@ -995,7 +995,7 @@
       </c>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="5">
         <v>2</v>
       </c>
@@ -1025,7 +1025,7 @@
       </c>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
         <v>2</v>
       </c>
@@ -1055,7 +1055,7 @@
       </c>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
         <v>2</v>
       </c>
@@ -1085,7 +1085,7 @@
       </c>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="5">
         <v>2</v>
       </c>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="5">
         <v>2</v>
       </c>
@@ -1145,7 +1145,7 @@
       </c>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="5">
         <v>2</v>
       </c>
@@ -1174,7 +1174,7 @@
         <v>0.44236111111111115</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="5">
         <v>2</v>
       </c>
@@ -1203,7 +1203,7 @@
         <v>0.44375000000000003</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="5">
         <v>2</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>0.44513888888888897</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="5">
         <v>2</v>
       </c>
@@ -1261,7 +1261,7 @@
         <v>0.44652777777777802</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="5">
         <v>2</v>
       </c>
@@ -1290,7 +1290,7 @@
         <v>0.44791666666666702</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="5">
         <v>2</v>
       </c>
@@ -1319,7 +1319,7 @@
         <v>0.52777777777777779</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="5">
         <v>2</v>
       </c>
@@ -1348,7 +1348,7 @@
         <v>0.52916666666666667</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="5">
         <v>2</v>
       </c>
@@ -1377,7 +1377,7 @@
         <v>0.53055555555555556</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="5">
         <v>2</v>
       </c>
@@ -1406,7 +1406,7 @@
         <v>0.53194444444444444</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="5">
         <v>2</v>
       </c>
@@ -1435,7 +1435,7 @@
         <v>0.53333333333333333</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="5">
         <v>2</v>
       </c>
@@ -1464,7 +1464,7 @@
         <v>0.53472222222222221</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="5">
         <v>2</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>0.53611111111111098</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="5">
         <v>2</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>0.53749999999999998</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="5">
         <v>2</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>0.53888888888888897</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="5">
         <v>2</v>
       </c>
@@ -1580,7 +1580,7 @@
         <v>0.54027777777777797</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="5">
         <v>2</v>
       </c>
@@ -1609,7 +1609,7 @@
         <v>0.54166666666666696</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="5">
         <v>2</v>
       </c>
@@ -1638,7 +1638,7 @@
         <v>0.54305555555555596</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="5">
         <v>2</v>
       </c>
@@ -1667,7 +1667,7 @@
         <v>0.54444444444444395</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="5">
         <v>2</v>
       </c>
@@ -1696,7 +1696,7 @@
         <v>0.54583333333333295</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="5">
         <v>2</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>0.54722222222222205</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="5">
         <v>2</v>
       </c>
@@ -1754,7 +1754,7 @@
         <v>0.54861111111111105</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="5">
         <v>2</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="5">
         <v>2</v>
       </c>
@@ -1812,7 +1812,7 @@
         <v>0.55138888888888904</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="5">
         <v>2</v>
       </c>
@@ -1841,7 +1841,7 @@
         <v>0.55277777777777803</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="5">
         <v>2</v>
       </c>
@@ -1870,7 +1870,7 @@
         <v>0.55416666666666703</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="5">
         <v>2</v>
       </c>
@@ -1899,7 +1899,7 @@
         <v>0.63194444444444442</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="5">
         <v>2</v>
       </c>
@@ -1928,7 +1928,7 @@
         <v>0.6333333333333333</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="5">
         <v>2</v>
       </c>
@@ -1957,7 +1957,7 @@
         <v>0.63472222222222219</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="5">
         <v>2</v>
       </c>
@@ -1986,7 +1986,7 @@
         <v>0.63611111111111096</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="5">
         <v>2</v>
       </c>
@@ -2015,7 +2015,7 @@
         <v>0.63749999999999996</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="5">
         <v>2</v>
       </c>
@@ -2044,7 +2044,7 @@
         <v>0.63888888888888895</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="5">
         <v>2</v>
       </c>
@@ -2073,7 +2073,7 @@
         <v>0.64027777777777795</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="5">
         <v>2</v>
       </c>
@@ -2102,7 +2102,7 @@
         <v>0.64166666666666705</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="5">
         <v>2</v>
       </c>
@@ -2131,7 +2131,7 @@
         <v>0.64305555555555505</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="5">
         <v>2</v>
       </c>
@@ -2160,7 +2160,7 @@
         <v>0.64444444444444404</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="5">
         <v>2</v>
       </c>
@@ -2189,7 +2189,7 @@
         <v>0.64583333333333304</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="5">
         <v>2</v>
       </c>
@@ -2218,7 +2218,7 @@
         <v>0.64722222222222203</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="5">
         <v>2</v>
       </c>
@@ -2247,7 +2247,7 @@
         <v>0.64861111111111103</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="5">
         <v>2</v>
       </c>
@@ -2276,7 +2276,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="5">
         <v>2</v>
       </c>
@@ -2305,7 +2305,7 @@
         <v>0.65138888888888902</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="5">
         <v>2</v>
       </c>
@@ -2334,7 +2334,7 @@
         <v>0.65277777777777801</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="5">
         <v>2</v>
       </c>
@@ -2363,7 +2363,7 @@
         <v>0.65416666666666701</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="5">
         <v>2</v>
       </c>
@@ -2392,7 +2392,7 @@
         <v>0.655555555555555</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="5">
         <v>2</v>
       </c>
@@ -2421,7 +2421,7 @@
         <v>0.656944444444444</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="5">
         <v>2</v>
       </c>
@@ -2450,7 +2450,7 @@
         <v>0.65833333333333299</v>
       </c>
     </row>
-    <row r="1048465" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="1048465" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G1048465" s="1"/>
     </row>
   </sheetData>

</xml_diff>